<commit_message>
added NAAQS and WHO standards, conversion to ug/m3
</commit_message>
<xml_diff>
--- a/arduino+esp01/DSM501A ratio to mg-m3.xlsx
+++ b/arduino+esp01/DSM501A ratio to mg-m3.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\GitHub\esp-8266\ESP-8266-particle-sensor\arduino+esp01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pcs per 0.01ft3" sheetId="2" r:id="rId1"/>
     <sheet name="DSM501A ratio to mg-m3" sheetId="1" r:id="rId2"/>
     <sheet name="Resistors for v1 output" sheetId="3" r:id="rId3"/>
+    <sheet name="convert part-ft3 to ug-m3" sheetId="4" r:id="rId4"/>
+    <sheet name="limits for exposure" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>mg/m3</t>
   </si>
@@ -60,6 +62,111 @@
   </si>
   <si>
     <t>27k</t>
+  </si>
+  <si>
+    <t>y = 4E-16x4 – 2E-11x3 + 3E-07x2 + 0.0014x + 1.9915</t>
+  </si>
+  <si>
+    <t>from aircasting thesis https://dl.dropboxusercontent.com/u/29720355/Besser%20Thesis%20FINAL.pdf</t>
+  </si>
+  <si>
+    <t>using shinyei ppd60v t2</t>
+  </si>
+  <si>
+    <t>http://www.pmeasuring.com/wrap/filesApp/BasicGuide/file_1/ver_1317144880/basicguide.pdf</t>
+  </si>
+  <si>
+    <t>Subsequent particle studies have shown distributions for airborne particles proportional to 1/(diameter)^2.1.</t>
+  </si>
+  <si>
+    <t>(number of particles &gt; 1 µm)* [1/(ratio of particle diameters)^2.1 ]</t>
+  </si>
+  <si>
+    <t>fair</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>very poor</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>dylos 1um</t>
+  </si>
+  <si>
+    <t>lower ug/m3</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>hunderds of particles per cubic foot, lower</t>
+  </si>
+  <si>
+    <t>US EPA NAAQS</t>
+  </si>
+  <si>
+    <t>24 hour period</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>very good</t>
+  </si>
+  <si>
+    <t>excellent</t>
+  </si>
+  <si>
+    <t>aircasting 2.5um</t>
+  </si>
+  <si>
+    <t>WHO 2.5um standards</t>
+  </si>
+  <si>
+    <t>http://www.who.int/mediacentre/factsheets/fs313/en/</t>
+  </si>
+  <si>
+    <t>http://www.epa.gov/air/criteria.html</t>
+  </si>
+  <si>
+    <t>24 hour</t>
+  </si>
+  <si>
+    <t>dylos 0.5um</t>
+  </si>
+  <si>
+    <t>http://www.epa.gov/airquality/particlepollution/2012/decfsstandards.pdf</t>
+  </si>
+  <si>
+    <t>hazardous</t>
+  </si>
+  <si>
+    <t>very unhealthy</t>
+  </si>
+  <si>
+    <t>unhealthy</t>
+  </si>
+  <si>
+    <t>unhealthy for sensitive groups</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>very hazardous</t>
+  </si>
+  <si>
+    <t>particle size 1</t>
+  </si>
+  <si>
+    <t>size 2</t>
+  </si>
+  <si>
+    <t>conversion factor</t>
   </si>
 </sst>
 </file>
@@ -618,7 +725,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -705,7 +811,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -788,11 +893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-12724048"/>
-        <c:axId val="-12723504"/>
+        <c:axId val="779266656"/>
+        <c:axId val="779267744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-12724048"/>
+        <c:axId val="779266656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,12 +954,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-12723504"/>
+        <c:crossAx val="779267744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-12723504"/>
+        <c:axId val="779267744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +1016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-12724048"/>
+        <c:crossAx val="779266656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -975,7 +1080,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1061,7 +1165,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1168,11 +1271,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1971872816"/>
-        <c:axId val="-1971883152"/>
+        <c:axId val="779268288"/>
+        <c:axId val="779272640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1971872816"/>
+        <c:axId val="779268288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,12 +1332,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1971883152"/>
+        <c:crossAx val="779272640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1971883152"/>
+        <c:axId val="779272640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1971872816"/>
+        <c:crossAx val="779268288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3116,7 +3219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3157,4 +3260,527 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>1/((A16/B16)^2.1)</f>
+        <v>4.2870938501451725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>7500</v>
+      </c>
+      <c r="D2">
+        <f>4*10^-16*B2^4 - 0.00000000002*B2^3 + 0.0000003*B2^2 + 0.0014*B2 + 1.9915</f>
+        <v>22.194624999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <v>7500</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:E5" si="0">4*10^-16*B3^4 - 0.00000000002*B3^3 + 0.0000003*B3^2 + 0.0014*B3 + 1.9915</f>
+        <v>14.2415</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>22.194624999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>2500</v>
+      </c>
+      <c r="C4">
+        <v>5000</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>7.0696250000000003</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>14.2415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>2500</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.0696250000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <f>B8*4.28/100</f>
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>350</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:E13" si="1">B9*4.28/100</f>
+        <v>14.98</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>350</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>4.28</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.14</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1.07</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>3000</v>
+      </c>
+      <c r="D16">
+        <f>B16/100</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1050</v>
+      </c>
+      <c r="C17">
+        <v>3000</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:E21" si="2">B17/100</f>
+        <v>10.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>1050</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>150</v>
+      </c>
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28">
+        <v>250</v>
+      </c>
+      <c r="E28">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>150</v>
+      </c>
+      <c r="E29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>55</v>
+      </c>
+      <c r="E30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>35</v>
+      </c>
+      <c r="E31">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more data on thresholds
</commit_message>
<xml_diff>
--- a/arduino+esp01/DSM501A ratio to mg-m3.xlsx
+++ b/arduino+esp01/DSM501A ratio to mg-m3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pcs per 0.01ft3" sheetId="2" r:id="rId1"/>
@@ -3266,7 +3266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -3338,7 +3338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>